<commit_message>
pubkeys removed for tests
</commit_message>
<xml_diff>
--- a/tests/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/tests/examples_for_test/print_lab_test/sampledata.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -347,15 +347,6 @@
   </si>
   <si>
     <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93B72373820DDB104BC6859474CBFBAB503F3CF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">james love</t>
-  </si>
-  <si>
-    <t xml:space="preserve">james.love@auckland.ac.nz</t>
   </si>
 </sst>
 </file>
@@ -618,7 +609,7 @@
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="2:2 E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3838,7 +3829,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="2:2 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3961,7 +3952,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="2:2 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4031,7 +4022,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4128,7 +4119,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4209,7 +4200,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="2:2 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4236,13 +4227,16 @@
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="8" t="b">
+      <c r="B2" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="b">
+      <c r="C2" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="b">
+      <c r="D2" s="8" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -4250,13 +4244,16 @@
       <c r="A3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="8" t="b">
+      <c r="B3" s="8" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="b">
+      <c r="C3" s="8" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="b">
+      <c r="D3" s="8" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -4264,13 +4261,16 @@
       <c r="A4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="8" t="b">
+      <c r="B4" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="b">
+      <c r="C4" s="8" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="b">
+      <c r="D4" s="8" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -4293,7 +4293,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4321,23 +4321,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>108</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="james.love@auckland.ac.nz"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
force gpg key for MyTardis user
</commit_message>
<xml_diff>
--- a/tests/examples_for_test/print_lab_test/sampledata.xlsx
+++ b/tests/examples_for_test/print_lab_test/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
   <si>
     <t xml:space="preserve">Sample name</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t xml:space="preserve">A006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NHI0000</t>
   </si>
   <si>
     <t xml:space="preserve">Male</t>
@@ -609,7 +606,7 @@
   <dimension ref="A1:XFD1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="2:2 E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3829,7 +3826,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="2:2 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3951,8 +3948,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="2:2 D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3987,17 +3984,13 @@
       <c r="B2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>32</v>
@@ -4022,7 +4015,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4033,71 +4026,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -4119,7 +4112,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4129,24 +4122,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>49</v>
@@ -4155,15 +4148,15 @@
         <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>57</v>
@@ -4172,10 +4165,10 @@
         <v>58</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4200,7 +4193,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="2:2 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4211,21 +4204,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="8" t="n">
         <f aca="false">FALSE()</f>
@@ -4242,7 +4235,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="8" t="n">
         <f aca="false">TRUE()</f>
@@ -4259,7 +4252,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="8" t="n">
         <f aca="false">FALSE()</f>
@@ -4292,8 +4285,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4305,19 +4298,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>